<commit_message>
Added parameter to enable/disable reading hidden rows/columns in Excel
</commit_message>
<xml_diff>
--- a/tst/Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests/TestUtilities/Files/TestFileMiscellaneous.xlsx
+++ b/tst/Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests/TestUtilities/Files/TestFileMiscellaneous.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmarcos\OneDrive - ENCAMINA S.L\Documentos\GitHub\enmarcha\tst\Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests\TestUtilities\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DB395C-3FFF-4EC8-8015-FBAD9D98875C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8C91D-D895-4417-B6B7-C19FC4E0058F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="2850" windowWidth="29040" windowHeight="15720" xr2:uid="{541DEC60-73F4-456F-8C96-E858248F8A75}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>